<commit_message>
Updated reference values, maybe wrong though
</commit_message>
<xml_diff>
--- a/src/text_files_for_read/Inputs.xlsx
+++ b/src/text_files_for_read/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/text_files_for_read/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9138FB3-69E4-7046-893B-934145960A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21BEC08-095F-6045-9973-2B2E365B20E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="1320" windowWidth="17260" windowHeight="15800" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="100" yWindow="800" windowWidth="28800" windowHeight="16680" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,15 @@
     <sheet name="README" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Active!$B$81,Active!$B$86,Active!$B$88,Active!$B$89</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Active!$B$74,Active!$B$79,Active!$B$81,Active!$B$82</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Active!$B$92</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Active!$F$59</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Active!$F$60</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Active!$B$85</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Active!$F$52</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Active!$F$53</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Active!$F$58</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Active!$F$51</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
@@ -688,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39602BD4-AF2D-864A-8905-789D980EB8BD}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1442,10 +1442,13 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="E22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="E23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1457,88 +1460,46 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="10"/>
+      <c r="B25" s="9"/>
       <c r="E25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="10"/>
+      <c r="B26" s="9"/>
       <c r="E26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="9"/>
       <c r="E27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="9"/>
       <c r="E28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="10"/>
       <c r="E29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="10"/>
       <c r="E30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B31" s="10"/>
       <c r="E31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B32" s="9"/>
       <c r="E32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="9"/>
-      <c r="E33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
switched neutrons/protons integration to LSD format, updated ref
</commit_message>
<xml_diff>
--- a/src/text_files_for_read/Inputs.xlsx
+++ b/src/text_files_for_read/Inputs.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/text_files_for_read/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21BEC08-095F-6045-9973-2B2E365B20E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581037AF-C11D-FC4D-84A3-36FF1BD99B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="800" windowWidth="28800" windowHeight="16680" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="32440" yWindow="2140" windowWidth="28800" windowHeight="16680" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
-    <sheet name="Sinclair" sheetId="3" r:id="rId2"/>
-    <sheet name="Evenstar" sheetId="2" r:id="rId3"/>
-    <sheet name="README" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Sinclair" sheetId="3" r:id="rId3"/>
+    <sheet name="Evenstar" sheetId="2" r:id="rId4"/>
+    <sheet name="README" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Active!$B$74,Active!$B$79,Active!$B$81,Active!$B$82</definedName>
@@ -46,9 +47,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -56,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
   <si>
     <t>Sample Name</t>
   </si>
@@ -233,6 +237,39 @@
   </si>
   <si>
     <t>code applies this value over the entire exposure duration</t>
+  </si>
+  <si>
+    <t>North Pole</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>NZ</t>
+  </si>
+  <si>
+    <t>South Pole</t>
   </si>
 </sst>
 </file>
@@ -360,10 +397,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -691,7 +728,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,16 +780,16 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="B2" s="9">
-        <v>-19.578942000000001</v>
+        <v>90</v>
       </c>
       <c r="C2" s="9">
-        <v>-69.872967000000003</v>
+        <v>0</v>
       </c>
       <c r="D2" s="9">
-        <v>1172</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
         <v>5</v>
@@ -778,16 +815,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="B3" s="10">
-        <v>-19.340944</v>
+        <v>75</v>
       </c>
       <c r="C3" s="10">
-        <v>-69.727999999999994</v>
-      </c>
-      <c r="D3" s="10">
-        <v>1607</v>
+        <v>-42</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0</v>
       </c>
       <c r="E3" s="1">
         <v>5</v>
@@ -813,16 +850,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="B4" s="10">
-        <v>-19.340944</v>
+        <v>60</v>
       </c>
       <c r="C4" s="10">
-        <v>-69.727999999999994</v>
-      </c>
-      <c r="D4" s="10">
-        <v>1607</v>
+        <v>18</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>5</v>
@@ -848,16 +885,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="B5" s="10">
-        <v>-19.340944</v>
+        <v>45</v>
       </c>
       <c r="C5" s="10">
-        <v>-69.727999999999994</v>
-      </c>
-      <c r="D5" s="10">
-        <v>1607</v>
+        <v>-95</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
       </c>
       <c r="E5" s="1">
         <v>5</v>
@@ -883,16 +920,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B6" s="10">
-        <v>-19.336722000000002</v>
+        <v>30</v>
       </c>
       <c r="C6" s="10">
-        <v>-69.729611000000006</v>
-      </c>
-      <c r="D6" s="10">
-        <v>1604</v>
+        <v>104</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
@@ -918,16 +955,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B7" s="9">
-        <v>-18.886583000000002</v>
+        <v>15</v>
       </c>
       <c r="C7" s="9">
-        <v>-69.699055999999999</v>
+        <v>-90</v>
       </c>
       <c r="D7" s="9">
-        <v>2282</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
@@ -953,16 +990,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B8" s="9">
-        <v>-18.886583000000002</v>
+        <v>0</v>
       </c>
       <c r="C8" s="9">
-        <v>-69.699055999999999</v>
+        <v>-78</v>
       </c>
       <c r="D8" s="9">
-        <v>2282</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
         <v>5</v>
@@ -988,16 +1025,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B9" s="9">
-        <v>-18.905639000000001</v>
+        <v>-15</v>
       </c>
       <c r="C9" s="9">
-        <v>-69.954583</v>
+        <v>46</v>
       </c>
       <c r="D9" s="9">
-        <v>1443</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
         <v>5</v>
@@ -1023,16 +1060,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B10" s="9">
-        <v>-18.905639000000001</v>
+        <v>-30</v>
       </c>
       <c r="C10" s="9">
-        <v>-69.954583</v>
+        <v>133</v>
       </c>
       <c r="D10" s="9">
-        <v>1443</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1">
         <v>5</v>
@@ -1058,16 +1095,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="B11" s="9">
-        <v>-18.852694</v>
+        <v>-45</v>
       </c>
       <c r="C11" s="9">
-        <v>-69.657167000000001</v>
+        <v>174</v>
       </c>
       <c r="D11" s="9">
-        <v>2550</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
         <v>5</v>
@@ -1093,16 +1130,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="B12" s="9">
-        <v>-20.704083000000001</v>
+        <v>-90</v>
       </c>
       <c r="C12" s="9">
-        <v>-69.420833000000002</v>
+        <v>0</v>
       </c>
       <c r="D12" s="9">
-        <v>1084</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1">
         <v>5</v>
@@ -1127,319 +1164,121 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="11">
-        <v>-19.786306</v>
-      </c>
-      <c r="C13" s="11">
-        <v>-69.682000000000002</v>
-      </c>
-      <c r="D13" s="11">
-        <v>1289</v>
-      </c>
-      <c r="E13" s="1">
-        <v>5</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="13">
-        <v>0</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="13"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="2">
-        <f>107.8*10^7</f>
-        <v>1078000000</v>
-      </c>
-      <c r="K13" s="2">
-        <f>2.77*10^7</f>
-        <v>27700000</v>
-      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="10">
-        <v>-19.786306</v>
-      </c>
-      <c r="C14" s="10">
-        <v>-69.682000000000002</v>
-      </c>
-      <c r="D14" s="10">
-        <v>1289</v>
-      </c>
-      <c r="E14" s="1">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="13">
-        <v>0</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="13"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="2">
-        <f>102.49*10^7</f>
-        <v>1024900000</v>
-      </c>
-      <c r="K14" s="2">
-        <f>2.48*10^7</f>
-        <v>24800000</v>
-      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="10">
-        <v>-19.786306</v>
-      </c>
-      <c r="C15" s="10">
-        <v>-69.682000000000002</v>
-      </c>
-      <c r="D15" s="10">
-        <v>1289</v>
-      </c>
-      <c r="E15" s="1">
-        <v>5</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="13">
-        <v>0</v>
-      </c>
+      <c r="A15" s="5"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="13"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="8">
-        <f>298.96*10^7</f>
-        <v>2989600000</v>
-      </c>
-      <c r="K15" s="2">
-        <f>3.2*10^7</f>
-        <v>32000000</v>
-      </c>
+      <c r="J15" s="8"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="10">
-        <v>-19.397832999999999</v>
-      </c>
-      <c r="C16" s="10">
-        <v>-69.880306000000004</v>
-      </c>
-      <c r="D16" s="10">
-        <v>1256</v>
-      </c>
-      <c r="E16" s="1">
-        <v>5</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="13">
-        <v>0</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="13"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="2">
-        <f>194.23*10^7</f>
-        <v>1942300000</v>
-      </c>
-      <c r="K16" s="2">
-        <f>4.67*10^7</f>
-        <v>46700000</v>
-      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="10">
-        <v>-19.397832999999999</v>
-      </c>
-      <c r="C17" s="10">
-        <v>-69.880306000000004</v>
-      </c>
-      <c r="D17" s="10">
-        <v>1256</v>
-      </c>
-      <c r="E17" s="1">
-        <v>5</v>
-      </c>
-      <c r="F17" s="1">
-        <v>2.74</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-      <c r="H17" s="13">
-        <v>0</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="13"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="2">
-        <f>310.26*10^7</f>
-        <v>3102600000</v>
-      </c>
-      <c r="K17" s="2">
-        <f>8.23*10^7</f>
-        <v>82300000</v>
-      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="10">
-        <v>-19.397832999999999</v>
-      </c>
-      <c r="C18" s="10">
-        <v>-69.880306000000004</v>
-      </c>
-      <c r="D18" s="10">
-        <v>1256</v>
-      </c>
-      <c r="E18" s="1">
-        <v>5</v>
-      </c>
-      <c r="F18" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-      <c r="H18" s="13">
-        <v>0</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="13"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="2">
-        <f>269.16*10^7</f>
-        <v>2691600000.0000005</v>
-      </c>
-      <c r="K18" s="2">
-        <f>6.18*10^7</f>
-        <v>61800000</v>
-      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="9">
-        <v>-19.522110999999999</v>
-      </c>
-      <c r="C19" s="9">
-        <v>-69.808333000000005</v>
-      </c>
-      <c r="D19" s="9">
-        <v>1312</v>
-      </c>
-      <c r="E19" s="1">
-        <v>5</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G19" s="1">
-        <v>1</v>
-      </c>
-      <c r="H19" s="13">
-        <v>0</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="13"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="2">
-        <f>277.15*10^7</f>
-        <v>2771500000</v>
-      </c>
-      <c r="K19" s="7">
-        <f>5.2*10^7</f>
-        <v>52000000</v>
-      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="9">
-        <v>-19.522110999999999</v>
-      </c>
-      <c r="C20" s="9">
-        <v>-69.808333000000005</v>
-      </c>
-      <c r="D20" s="9">
-        <v>1312</v>
-      </c>
-      <c r="E20" s="1">
-        <v>5</v>
-      </c>
-      <c r="F20" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
-      <c r="H20" s="13">
-        <v>0</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="2">
-        <f>65.4*10^7</f>
-        <v>654000000</v>
-      </c>
-      <c r="K20" s="7">
-        <f>1.5*10^7</f>
-        <v>15000000</v>
-      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="12">
-        <v>-18.503527999999999</v>
-      </c>
-      <c r="C21" s="12">
-        <v>-70.143305999999995</v>
-      </c>
-      <c r="D21" s="12">
-        <v>771</v>
-      </c>
-      <c r="E21" s="1">
-        <v>5</v>
-      </c>
-      <c r="F21" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" s="13">
-        <v>0</v>
-      </c>
+      <c r="A21" s="6"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="13"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="2">
-        <f>41.29*10^7</f>
-        <v>412900000</v>
-      </c>
-      <c r="K21" s="7">
-        <f>0.72*10^7</f>
-        <v>7200000</v>
-      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" s="10"/>
@@ -1508,6 +1347,406 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9FD288-F7FF-CC43-984C-6BC5F64D5A7D}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="9">
+        <v>90</v>
+      </c>
+      <c r="C1" s="9">
+        <v>0</v>
+      </c>
+      <c r="D1" s="9">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G1" s="1">
+        <v>1</v>
+      </c>
+      <c r="H1" s="13">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1">
+        <f>65.91*10^7</f>
+        <v>659100000</v>
+      </c>
+      <c r="K1" s="1">
+        <f>1.2*10^7</f>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="10">
+        <v>75</v>
+      </c>
+      <c r="C2" s="10">
+        <v>-42</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2">
+        <f>74.48*10^7</f>
+        <v>744800000</v>
+      </c>
+      <c r="K2" s="2">
+        <f>2.33*10^7</f>
+        <v>23300000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="10">
+        <v>60</v>
+      </c>
+      <c r="C3" s="10">
+        <v>18</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2">
+        <f>91.1*10^7</f>
+        <v>911000000</v>
+      </c>
+      <c r="K3" s="2">
+        <f>1.3*10^7</f>
+        <v>13000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="10">
+        <v>45</v>
+      </c>
+      <c r="C4" s="10">
+        <v>-95</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2">
+        <f>167.12*10^7</f>
+        <v>1671200000</v>
+      </c>
+      <c r="K4" s="2">
+        <f>3.65*10^7</f>
+        <v>36500000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="10">
+        <v>30</v>
+      </c>
+      <c r="C5" s="10">
+        <v>104</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2">
+        <f>104.68*10^7</f>
+        <v>1046800000.0000001</v>
+      </c>
+      <c r="K5" s="2">
+        <f>2.24*10^7</f>
+        <v>22400000.000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="9">
+        <v>15</v>
+      </c>
+      <c r="C6" s="9">
+        <v>-90</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2">
+        <f>269.89*10^7</f>
+        <v>2698900000</v>
+      </c>
+      <c r="K6" s="7">
+        <f>4.73*10^7</f>
+        <v>47300000.000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0</v>
+      </c>
+      <c r="C7" s="9">
+        <v>-78</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2">
+        <f>246.53*10^7</f>
+        <v>2465300000</v>
+      </c>
+      <c r="K7" s="7">
+        <f>4.29*10^7</f>
+        <v>42900000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="9">
+        <v>-15</v>
+      </c>
+      <c r="C8" s="9">
+        <v>46</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2">
+        <f>141.41*10^7</f>
+        <v>1414100000</v>
+      </c>
+      <c r="K8" s="7">
+        <f>2.52*10^7</f>
+        <v>25200000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="9">
+        <v>-30</v>
+      </c>
+      <c r="C9" s="9">
+        <v>133</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="2">
+        <f>164.8*10^7</f>
+        <v>1648000000</v>
+      </c>
+      <c r="K9" s="7">
+        <f>2.84*10^7</f>
+        <v>28400000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="9">
+        <v>-45</v>
+      </c>
+      <c r="C10" s="9">
+        <v>174</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="2">
+        <f>235*10^7</f>
+        <v>2350000000</v>
+      </c>
+      <c r="K10" s="7">
+        <f>4.04*10^7</f>
+        <v>40400000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="9">
+        <v>-90</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2">
+        <f>90.19*10^7</f>
+        <v>901900000</v>
+      </c>
+      <c r="K11" s="7">
+        <f>1.97*10^7</f>
+        <v>19700000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081048F5-9F92-C54B-B1C5-62D0C1F0285D}">
   <dimension ref="A1:K39"/>
   <sheetViews>
@@ -2248,7 +2487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1377A66-7F29-A649-8A24-0084E41BD032}">
   <dimension ref="A1:K21"/>
   <sheetViews>
@@ -2999,7 +3238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A252A25-C5BD-9644-90A1-8F508F9F4733}">
   <dimension ref="A1:K18"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated plotting script and long term average
</commit_message>
<xml_diff>
--- a/src/text_files_for_read/Inputs.xlsx
+++ b/src/text_files_for_read/Inputs.xlsx
@@ -8,36 +8,56 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/text_files_for_read/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581037AF-C11D-FC4D-84A3-36FF1BD99B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D7666E-DDA7-374E-B681-79B8A4255AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32440" yWindow="2140" windowWidth="28800" windowHeight="16680" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="560" yWindow="460" windowWidth="28800" windowHeight="16680" activeTab="1" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
-    <sheet name="Sinclair" sheetId="3" r:id="rId3"/>
-    <sheet name="Evenstar" sheetId="2" r:id="rId4"/>
-    <sheet name="README" sheetId="4" r:id="rId5"/>
+    <sheet name="Figure 2" sheetId="7" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Sinclair" sheetId="3" r:id="rId4"/>
+    <sheet name="Libarkin" sheetId="6" r:id="rId5"/>
+    <sheet name="Evenstar" sheetId="2" r:id="rId6"/>
+    <sheet name="README" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Active!$B$74,Active!$B$79,Active!$B$81,Active!$B$82</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Figure 2'!$B$74,'Figure 2'!$B$79,'Figure 2'!$B$81,'Figure 2'!$B$82</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Active!$B$85</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Figure 2'!$B$85</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Active!$F$52</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Figure 2'!$F$52</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Active!$F$53</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Figure 2'!$F$53</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Active!$F$51</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Figure 2'!$F$51</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0.4</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">0.4</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">1.4</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">1.4</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">98.2</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">98.2</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="82">
   <si>
     <t>Sample Name</t>
   </si>
@@ -270,6 +290,42 @@
   </si>
   <si>
     <t>South Pole</t>
+  </si>
+  <si>
+    <t>20A</t>
+  </si>
+  <si>
+    <t>22C</t>
+  </si>
+  <si>
+    <t>01A</t>
+  </si>
+  <si>
+    <t>01B</t>
+  </si>
+  <si>
+    <t>20F</t>
+  </si>
+  <si>
+    <t>21A</t>
+  </si>
+  <si>
+    <t>22D</t>
+  </si>
+  <si>
+    <t>27C</t>
+  </si>
+  <si>
+    <t>21ACR</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>Africa</t>
   </si>
 </sst>
 </file>
@@ -727,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39602BD4-AF2D-864A-8905-789D980EB8BD}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,13 +836,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="B2" s="9">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C2" s="9">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="D2" s="9">
         <v>0</v>
@@ -815,359 +871,163 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="10">
-        <v>75</v>
-      </c>
-      <c r="C3" s="10">
-        <v>-42</v>
+        <v>80</v>
+      </c>
+      <c r="B3" s="9">
+        <v>-19</v>
+      </c>
+      <c r="C3" s="9">
+        <v>-69</v>
       </c>
       <c r="D3" s="9">
         <v>0</v>
       </c>
-      <c r="E3" s="1">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13">
-        <v>0</v>
-      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="13"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="2">
-        <f>74.48*10^7</f>
-        <v>744800000</v>
-      </c>
-      <c r="K3" s="2">
-        <f>2.33*10^7</f>
-        <v>23300000</v>
-      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="10">
-        <v>60</v>
-      </c>
-      <c r="C4" s="10">
-        <v>18</v>
+        <v>79</v>
+      </c>
+      <c r="B4" s="9">
+        <v>75</v>
+      </c>
+      <c r="C4" s="9">
+        <v>-42</v>
       </c>
       <c r="D4" s="9">
         <v>0</v>
       </c>
-      <c r="E4" s="1">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0</v>
-      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="13"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="2">
-        <f>91.1*10^7</f>
-        <v>911000000</v>
-      </c>
-      <c r="K4" s="2">
-        <f>1.3*10^7</f>
-        <v>13000000</v>
-      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="10">
-        <v>45</v>
-      </c>
-      <c r="C5" s="10">
-        <v>-95</v>
+        <v>81</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9">
+        <v>20</v>
       </c>
       <c r="D5" s="9">
         <v>0</v>
       </c>
-      <c r="E5" s="1">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="13">
-        <v>0</v>
-      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="13"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="2">
-        <f>167.12*10^7</f>
-        <v>1671200000</v>
-      </c>
-      <c r="K5" s="2">
-        <f>3.65*10^7</f>
-        <v>36500000</v>
-      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="10">
-        <v>30</v>
-      </c>
-      <c r="C6" s="10">
-        <v>104</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="13">
-        <v>0</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="13"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="2">
-        <f>104.68*10^7</f>
-        <v>1046800000.0000001</v>
-      </c>
-      <c r="K6" s="2">
-        <f>2.24*10^7</f>
-        <v>22400000.000000004</v>
-      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="9">
-        <v>15</v>
-      </c>
-      <c r="C7" s="9">
-        <v>-90</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>5</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13">
-        <v>0</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="13"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="2">
-        <f>269.89*10^7</f>
-        <v>2698900000</v>
-      </c>
-      <c r="K7" s="7">
-        <f>4.73*10^7</f>
-        <v>47300000.000000007</v>
-      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="9">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9">
-        <v>-78</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="13">
-        <v>0</v>
-      </c>
+      <c r="A8" s="4"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="13"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="2">
-        <f>246.53*10^7</f>
-        <v>2465300000</v>
-      </c>
-      <c r="K8" s="7">
-        <f>4.29*10^7</f>
-        <v>42900000</v>
-      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="9">
-        <v>-15</v>
-      </c>
-      <c r="C9" s="9">
-        <v>46</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="13">
-        <v>0</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="13"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="2">
-        <f>141.41*10^7</f>
-        <v>1414100000</v>
-      </c>
-      <c r="K9" s="7">
-        <f>2.52*10^7</f>
-        <v>25200000</v>
-      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="9">
-        <v>-30</v>
-      </c>
-      <c r="C10" s="9">
-        <v>133</v>
-      </c>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>5</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="13">
-        <v>0</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="13"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="2">
-        <f>164.8*10^7</f>
-        <v>1648000000</v>
-      </c>
-      <c r="K10" s="7">
-        <f>2.84*10^7</f>
-        <v>28400000</v>
-      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="9">
-        <v>-45</v>
-      </c>
-      <c r="C11" s="9">
-        <v>174</v>
-      </c>
-      <c r="D11" s="9">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="13">
-        <v>0</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="13"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="2">
-        <f>235*10^7</f>
-        <v>2350000000</v>
-      </c>
-      <c r="K11" s="7">
-        <f>4.04*10^7</f>
-        <v>40400000</v>
-      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="9">
-        <v>-90</v>
-      </c>
-      <c r="C12" s="9">
-        <v>0</v>
-      </c>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>5</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="13">
-        <v>0</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="13"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="2">
-        <f>90.19*10^7</f>
-        <v>901900000</v>
-      </c>
-      <c r="K12" s="7">
-        <f>1.97*10^7</f>
-        <v>19700000</v>
-      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1178,9 +1038,9 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1191,9 +1051,9 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1204,9 +1064,9 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1217,9 +1077,9 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1230,9 +1090,9 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1269,9 +1129,9 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1347,11 +1207,437 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2CA47B-538E-684E-879A-957351F4517A}">
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9">
+        <v>20</v>
+      </c>
+      <c r="C2" s="9">
+        <v>73</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1">
+        <f>65.91*10^7</f>
+        <v>659100000</v>
+      </c>
+      <c r="K2" s="1">
+        <f>1.2*10^7</f>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="9">
+        <v>-19</v>
+      </c>
+      <c r="C3" s="9">
+        <v>-69</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="9">
+        <v>75</v>
+      </c>
+      <c r="C4" s="9">
+        <v>-42</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9">
+        <v>20</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="10"/>
+      <c r="E22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="10"/>
+      <c r="E23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="10"/>
+      <c r="E24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="9"/>
+      <c r="E25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="9"/>
+      <c r="E26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9FD288-F7FF-CC43-984C-6BC5F64D5A7D}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K11"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1746,7 +2032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081048F5-9F92-C54B-B1C5-62D0C1F0285D}">
   <dimension ref="A1:K39"/>
   <sheetViews>
@@ -2487,12 +2773,511 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC882D3-3A74-104E-AD7A-9ACBA6AE09B6}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="10">
+        <v>38</v>
+      </c>
+      <c r="C2" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E2" s="1">
+        <v>115</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2">
+        <v>2380000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>56000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="10">
+        <v>38</v>
+      </c>
+      <c r="C3" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D3" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E3" s="1">
+        <v>115</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2">
+        <v>2630000</v>
+      </c>
+      <c r="K3" s="7">
+        <v>59000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="10">
+        <v>38</v>
+      </c>
+      <c r="C4" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D4" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E4" s="1">
+        <v>115</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2">
+        <v>2750000</v>
+      </c>
+      <c r="K4" s="7">
+        <v>57000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="10">
+        <v>38</v>
+      </c>
+      <c r="C5" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E5" s="1">
+        <v>135</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2">
+        <v>33000</v>
+      </c>
+      <c r="K5" s="7">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="10">
+        <v>38</v>
+      </c>
+      <c r="C6" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E6" s="1">
+        <v>145</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2">
+        <v>73000</v>
+      </c>
+      <c r="K6" s="7">
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="10">
+        <v>38</v>
+      </c>
+      <c r="C7" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D7" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E7" s="1">
+        <v>135</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2">
+        <v>34000</v>
+      </c>
+      <c r="K7" s="7">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="10">
+        <v>38</v>
+      </c>
+      <c r="C8" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2">
+        <v>6920000</v>
+      </c>
+      <c r="K8" s="7">
+        <v>69000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="10">
+        <v>38</v>
+      </c>
+      <c r="C9" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D9" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E9" s="1">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="2">
+        <v>7590000</v>
+      </c>
+      <c r="K9" s="7">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="10">
+        <v>38</v>
+      </c>
+      <c r="C10" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D10" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E10" s="1">
+        <v>155</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="2">
+        <v>59000</v>
+      </c>
+      <c r="K10" s="7">
+        <v>56000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1377A66-7F29-A649-8A24-0084E41BD032}">
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD21"/>
+      <selection sqref="A1:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3238,7 +4023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A252A25-C5BD-9644-90A1-8F508F9F4733}">
   <dimension ref="A1:K18"/>
   <sheetViews>

</xml_diff>

<commit_message>
updating libarkin dataset test
</commit_message>
<xml_diff>
--- a/src/text_files_for_read/Inputs.xlsx
+++ b/src/text_files_for_read/Inputs.xlsx
@@ -8,57 +8,59 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/text_files_for_read/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD0D7D6-F7DB-9A4D-A6D4-14ECD4FEE2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F998443-FD33-7B4F-BE80-2D8C682B5B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18260" windowHeight="16680" activeTab="1" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
-    <sheet name="Figure 1" sheetId="8" r:id="rId2"/>
-    <sheet name="Figure 3" sheetId="7" r:id="rId3"/>
-    <sheet name="Figure 6" sheetId="5" r:id="rId4"/>
-    <sheet name="Sinclair" sheetId="3" r:id="rId5"/>
-    <sheet name="Libarkin" sheetId="6" r:id="rId6"/>
-    <sheet name="Evenstar" sheetId="2" r:id="rId7"/>
-    <sheet name="README" sheetId="4" r:id="rId8"/>
+    <sheet name="Libarkin" sheetId="11" r:id="rId2"/>
+    <sheet name="SPICE" sheetId="9" r:id="rId3"/>
+    <sheet name="Figure 2" sheetId="10" r:id="rId4"/>
+    <sheet name="Figure 1" sheetId="8" r:id="rId5"/>
+    <sheet name="Figure 3" sheetId="7" r:id="rId6"/>
+    <sheet name="Figure 6" sheetId="5" r:id="rId7"/>
+    <sheet name="Sinclair" sheetId="3" r:id="rId8"/>
+    <sheet name="Evenstar" sheetId="2" r:id="rId9"/>
+    <sheet name="README" sheetId="4" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Active!$B$73,Active!$B$78,Active!$B$80,Active!$B$81</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">'Figure 3'!$B$74,'Figure 3'!$B$79,'Figure 3'!$B$81,'Figure 3'!$B$82</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Active!$B$74,Active!$B$79,Active!$B$81,Active!$B$82</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">'Figure 3'!$B$74,'Figure 3'!$B$79,'Figure 3'!$B$81,'Figure 3'!$B$82</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Active!$B$84</definedName>
-    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Figure 3'!$B$85</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Active!$F$51</definedName>
-    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Figure 3'!$F$52</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Active!$F$52</definedName>
-    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Figure 3'!$F$53</definedName>
+    <definedName name="solver_eng" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Active!$B$85</definedName>
+    <definedName name="solver_lhs1" localSheetId="5" hidden="1">'Figure 3'!$B$85</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Active!$F$52</definedName>
+    <definedName name="solver_lhs2" localSheetId="5" hidden="1">'Figure 3'!$F$52</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Active!$F$53</definedName>
+    <definedName name="solver_lhs3" localSheetId="5" hidden="1">'Figure 3'!$F$53</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_lin" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Active!$F$50</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">'Figure 3'!$F$51</definedName>
+    <definedName name="solver_num" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Active!$F$51</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">'Figure 3'!$F$51</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel3" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="5" hidden="1">2</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_rhs1" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_rhs1" localSheetId="5" hidden="1">100</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0.4</definedName>
-    <definedName name="solver_rhs2" localSheetId="2" hidden="1">0.4</definedName>
+    <definedName name="solver_rhs2" localSheetId="5" hidden="1">0.4</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">1.4</definedName>
-    <definedName name="solver_rhs3" localSheetId="2" hidden="1">1.4</definedName>
+    <definedName name="solver_rhs3" localSheetId="5" hidden="1">1.4</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_typ" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_typ" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">98.2</definedName>
-    <definedName name="solver_val" localSheetId="2" hidden="1">98.2</definedName>
+    <definedName name="solver_val" localSheetId="5" hidden="1">98.2</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="5" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -81,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="82">
   <si>
     <t>Sample Name</t>
   </si>
@@ -248,9 +250,6 @@
     <t>put 1 if no shielding</t>
   </si>
   <si>
-    <t>0&lt;=x&lt;=1</t>
-  </si>
-  <si>
     <t>from CRONUS</t>
   </si>
   <si>
@@ -266,12 +265,6 @@
     <t>22C</t>
   </si>
   <si>
-    <t>01A</t>
-  </si>
-  <si>
-    <t>01B</t>
-  </si>
-  <si>
     <t>20F</t>
   </si>
   <si>
@@ -312,13 +305,37 @@
   </si>
   <si>
     <t>21-12</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>10SPC01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -365,6 +382,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF2E2E2E"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -410,7 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,6 +473,10 @@
     </xf>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -767,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39602BD4-AF2D-864A-8905-789D980EB8BD}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -822,7 +849,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="10">
         <v>38</v>
@@ -834,7 +861,7 @@
         <v>2500</v>
       </c>
       <c r="E2" s="1">
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1">
         <v>2.3199999999999998</v>
@@ -843,7 +870,8 @@
         <v>1</v>
       </c>
       <c r="H2" s="13">
-        <v>0</v>
+        <f>10^-6</f>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="2">
@@ -855,7 +883,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" s="10">
         <v>38</v>
@@ -867,7 +895,7 @@
         <v>2500</v>
       </c>
       <c r="E3" s="1">
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1">
         <v>2.3199999999999998</v>
@@ -876,7 +904,8 @@
         <v>1</v>
       </c>
       <c r="H3" s="13">
-        <v>0</v>
+        <f t="shared" ref="H3:H8" si="0">10^-6</f>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="2">
@@ -888,7 +917,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B4" s="10">
         <v>38</v>
@@ -900,7 +929,7 @@
         <v>2500</v>
       </c>
       <c r="E4" s="1">
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1">
         <v>2.3199999999999998</v>
@@ -909,7 +938,8 @@
         <v>1</v>
       </c>
       <c r="H4" s="13">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="2">
@@ -921,7 +951,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="10">
         <v>38</v>
@@ -933,7 +963,7 @@
         <v>2500</v>
       </c>
       <c r="E5" s="1">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="F5" s="1">
         <v>2.3199999999999998</v>
@@ -942,7 +972,8 @@
         <v>1</v>
       </c>
       <c r="H5" s="13">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="2">
@@ -954,7 +985,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B6" s="10">
         <v>38</v>
@@ -966,7 +997,7 @@
         <v>2500</v>
       </c>
       <c r="E6" s="1">
-        <v>145</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1">
         <v>2.3199999999999998</v>
@@ -975,7 +1006,8 @@
         <v>1</v>
       </c>
       <c r="H6" s="13">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="2">
@@ -987,7 +1019,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B7" s="10">
         <v>38</v>
@@ -999,7 +1031,7 @@
         <v>2500</v>
       </c>
       <c r="E7" s="1">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1">
         <v>2.3199999999999998</v>
@@ -1008,7 +1040,8 @@
         <v>1</v>
       </c>
       <c r="H7" s="13">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="2">
@@ -1019,8 +1052,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>61</v>
+      <c r="A8" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="B8" s="10">
         <v>38</v>
@@ -1032,7 +1065,7 @@
         <v>2500</v>
       </c>
       <c r="E8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" s="1">
         <v>2.3199999999999998</v>
@@ -1041,81 +1074,42 @@
         <v>1</v>
       </c>
       <c r="H8" s="13">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="2">
-        <v>6920000</v>
+        <v>59000</v>
       </c>
       <c r="K8" s="7">
-        <v>69000</v>
+        <v>56000</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="10">
-        <v>38</v>
-      </c>
-      <c r="C9" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D9" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E9" s="1">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="13">
-        <v>0</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="13"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="2">
-        <v>7590000</v>
-      </c>
-      <c r="K9" s="7">
-        <v>31000</v>
-      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="10">
-        <v>38</v>
-      </c>
-      <c r="C10" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D10" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E10" s="1">
-        <v>155</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="13">
-        <v>0</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="13"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="2">
-        <v>59000</v>
-      </c>
-      <c r="K10" s="7">
-        <v>56000</v>
-      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
@@ -1131,23 +1125,23 @@
       <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="13"/>
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1157,7 +1151,7 @@
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
+      <c r="A14" s="1"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -1166,11 +1160,11 @@
       <c r="G14" s="1"/>
       <c r="H14" s="13"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="8"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -1179,7 +1173,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="13"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="2"/>
+      <c r="J15" s="8"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1209,17 +1203,17 @@
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="13"/>
       <c r="I18" s="1"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="7"/>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
@@ -1235,10 +1229,10 @@
       <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1248,10 +1242,17 @@
       <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="10"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="13"/>
       <c r="I21" s="1"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" s="10"/>
@@ -1266,7 +1267,7 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="9"/>
+      <c r="B24" s="10"/>
       <c r="E24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1278,16 +1279,19 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="9"/>
       <c r="E26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="9"/>
       <c r="E27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="9"/>
       <c r="E28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -1306,6 +1310,11 @@
       <c r="E31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -1313,12 +1322,381 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A252A25-C5BD-9644-90A1-8F508F9F4733}">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="14">
+        <v>6300000</v>
+      </c>
+      <c r="K2" s="14">
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="14">
+        <v>27600000</v>
+      </c>
+      <c r="K3" s="14">
+        <v>2100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="14">
+        <v>35700000</v>
+      </c>
+      <c r="K4" s="14">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="14">
+        <v>2300000</v>
+      </c>
+      <c r="K5" s="14">
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="14">
+        <v>313000000</v>
+      </c>
+      <c r="K6" s="14">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="14">
+        <v>37300000</v>
+      </c>
+      <c r="K7" s="14">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="14">
+        <v>1270000</v>
+      </c>
+      <c r="K8" s="14">
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="14">
+        <v>27100000</v>
+      </c>
+      <c r="K9" s="14">
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="14">
+        <v>55100000</v>
+      </c>
+      <c r="K10" s="14">
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="14">
+        <v>17700000</v>
+      </c>
+      <c r="K11" s="14">
+        <v>950000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="14">
+        <v>9100000</v>
+      </c>
+      <c r="K12" s="14">
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="14">
+        <v>2400000</v>
+      </c>
+      <c r="K13" s="14">
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="14">
+        <v>6200000</v>
+      </c>
+      <c r="K14" s="14">
+        <v>1400000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="14">
+        <v>53600000</v>
+      </c>
+      <c r="K15" s="14">
+        <v>2600000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="14">
+        <v>19900000</v>
+      </c>
+      <c r="K16" s="14">
+        <v>1700000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="14">
+        <v>45700000</v>
+      </c>
+      <c r="K17" s="14">
+        <v>2300000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="14">
+        <v>118000000</v>
+      </c>
+      <c r="K18" s="14">
+        <v>4700000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0692F123-E8ED-A84F-B1D6-10660BCC4234}">
-  <dimension ref="A1:K13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24694F2A-853A-E44C-A507-6368D3EEDD55}">
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1357,6 +1735,869 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="10">
+        <v>38</v>
+      </c>
+      <c r="C2" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <f>10^-6</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2">
+        <v>2380000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>56000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="10">
+        <v>38</v>
+      </c>
+      <c r="C3" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D3" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <f t="shared" ref="H3:H8" si="0">10^-6</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2">
+        <v>2630000</v>
+      </c>
+      <c r="K3" s="7">
+        <v>59000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="10">
+        <v>38</v>
+      </c>
+      <c r="C4" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D4" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2">
+        <v>2750000</v>
+      </c>
+      <c r="K4" s="7">
+        <v>57000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="10">
+        <v>38</v>
+      </c>
+      <c r="C5" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2">
+        <v>33000</v>
+      </c>
+      <c r="K5" s="7">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="10">
+        <v>38</v>
+      </c>
+      <c r="C6" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2">
+        <v>73000</v>
+      </c>
+      <c r="K6" s="7">
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="10">
+        <v>38</v>
+      </c>
+      <c r="C7" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D7" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2">
+        <v>34000</v>
+      </c>
+      <c r="K7" s="7">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="10">
+        <v>38</v>
+      </c>
+      <c r="C8" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2">
+        <v>59000</v>
+      </c>
+      <c r="K8" s="7">
+        <v>56000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D985B3A1-D71F-474D-89CB-3BE7E854D433}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="15">
+        <v>35.5944</v>
+      </c>
+      <c r="C2" s="15">
+        <v>111.63420000000001</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1837</v>
+      </c>
+      <c r="E2" s="15">
+        <v>8</v>
+      </c>
+      <c r="F2" s="15">
+        <v>2.25</v>
+      </c>
+      <c r="G2" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0</v>
+      </c>
+      <c r="J2" s="15">
+        <f>4.09*10^6</f>
+        <v>4090000</v>
+      </c>
+      <c r="K2">
+        <f>0.45*10^6</f>
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="15">
+        <v>35.605600000000003</v>
+      </c>
+      <c r="C3" s="15">
+        <v>111.61750000000001</v>
+      </c>
+      <c r="D3" s="15">
+        <v>1807</v>
+      </c>
+      <c r="E3" s="15">
+        <v>8</v>
+      </c>
+      <c r="F3" s="15">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="G3" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="H3" s="15">
+        <v>0</v>
+      </c>
+      <c r="J3" s="15">
+        <f>4.42*10^6</f>
+        <v>4420000</v>
+      </c>
+      <c r="K3">
+        <f>0.44*10^6</f>
+        <v>440000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="15">
+        <v>35.61</v>
+      </c>
+      <c r="C4" s="15">
+        <v>111.61369999999999</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1810</v>
+      </c>
+      <c r="E4" s="15">
+        <v>13</v>
+      </c>
+      <c r="F4" s="15">
+        <v>3.15</v>
+      </c>
+      <c r="G4" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="H4" s="15">
+        <v>0</v>
+      </c>
+      <c r="J4" s="15">
+        <f>4.17*10^6</f>
+        <v>4170000</v>
+      </c>
+      <c r="K4">
+        <f>0.39*10^6</f>
+        <v>390000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="15">
+        <v>35.616300000000003</v>
+      </c>
+      <c r="C5" s="15">
+        <v>111.60809999999999</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1800</v>
+      </c>
+      <c r="E5" s="15">
+        <v>13</v>
+      </c>
+      <c r="F5" s="15">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="G5" s="15">
+        <v>1</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0</v>
+      </c>
+      <c r="J5" s="15">
+        <f>4.16*10^6</f>
+        <v>4160000</v>
+      </c>
+      <c r="K5">
+        <f>0.46*10^6</f>
+        <v>460000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="15">
+        <v>35.624499999999998</v>
+      </c>
+      <c r="C6" s="15">
+        <v>111.6057</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1778</v>
+      </c>
+      <c r="E6" s="15">
+        <v>13</v>
+      </c>
+      <c r="F6" s="15">
+        <v>2.29</v>
+      </c>
+      <c r="G6" s="15">
+        <v>1</v>
+      </c>
+      <c r="H6" s="15">
+        <v>0</v>
+      </c>
+      <c r="J6" s="15">
+        <f>3.9*10^6</f>
+        <v>3900000</v>
+      </c>
+      <c r="K6">
+        <f>0.45*10^6</f>
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="15">
+        <v>35.616399999999999</v>
+      </c>
+      <c r="C7" s="15">
+        <v>111.6087</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1800</v>
+      </c>
+      <c r="E7" s="15">
+        <v>13</v>
+      </c>
+      <c r="F7" s="15">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="G7" s="15">
+        <v>1</v>
+      </c>
+      <c r="H7" s="15">
+        <v>0</v>
+      </c>
+      <c r="J7" s="15">
+        <f>4.02*10^6</f>
+        <v>4019999.9999999995</v>
+      </c>
+      <c r="K7">
+        <f>0.52*10^6</f>
+        <v>520000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="15">
+        <v>35.609400000000001</v>
+      </c>
+      <c r="C8" s="15">
+        <v>111.6135</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1810</v>
+      </c>
+      <c r="E8" s="15">
+        <v>13</v>
+      </c>
+      <c r="F8" s="15">
+        <v>2.29</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="H8" s="15">
+        <v>0</v>
+      </c>
+      <c r="J8" s="15">
+        <f>4.17*10^6</f>
+        <v>4170000</v>
+      </c>
+      <c r="K8">
+        <f>0.66*10^6</f>
+        <v>660000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="15">
+        <v>35.587800000000001</v>
+      </c>
+      <c r="C9" s="15">
+        <v>111.6345</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1876</v>
+      </c>
+      <c r="E9" s="15">
+        <v>6</v>
+      </c>
+      <c r="F9" s="15">
+        <v>2.25</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="J9" s="15">
+        <f>4.36*10^6</f>
+        <v>4360000</v>
+      </c>
+      <c r="K9">
+        <f>0.47*10^6</f>
+        <v>470000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345E843F-B5AF-7544-9892-CA1AD39C5E9D}">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>35</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>55</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>60</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>65</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>70</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>75</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>80</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>85</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>90</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0692F123-E8ED-A84F-B1D6-10660BCC4234}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="9">
@@ -1497,7 +2738,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B6" s="9">
         <v>90</v>
@@ -1523,7 +2764,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B7" s="10">
         <v>0</v>
@@ -1549,7 +2790,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B8" s="10">
         <v>90</v>
@@ -1575,7 +2816,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B9" s="10">
         <v>0</v>
@@ -1601,7 +2842,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B10" s="9">
         <v>90</v>
@@ -1665,7 +2906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2CA47B-538E-684E-879A-957351F4517A}">
   <dimension ref="A1:K32"/>
   <sheetViews>
@@ -1757,7 +2998,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3" s="9">
         <v>-19</v>
@@ -1778,7 +3019,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" s="9">
         <v>75</v>
@@ -1799,7 +3040,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B5" s="9">
         <v>0</v>
@@ -2091,12 +3332,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9FD288-F7FF-CC43-984C-6BC5F64D5A7D}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="A2" sqref="A2:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2135,7 +3376,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2" s="9">
         <v>75</v>
@@ -2149,7 +3390,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B3" s="9">
         <v>75</v>
@@ -2163,7 +3404,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" s="9">
         <v>75</v>
@@ -2177,7 +3418,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B5" s="9">
         <v>75</v>
@@ -2191,7 +3432,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B6" s="9">
         <v>75</v>
@@ -2205,7 +3446,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B7" s="9">
         <v>0</v>
@@ -2219,7 +3460,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B8" s="9">
         <v>0</v>
@@ -2233,7 +3474,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B9" s="9">
         <v>0</v>
@@ -2247,7 +3488,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B10" s="9">
         <v>0</v>
@@ -2261,7 +3502,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B11" s="9">
         <v>0</v>
@@ -2278,7 +3519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081048F5-9F92-C54B-B1C5-62D0C1F0285D}">
   <dimension ref="A1:K39"/>
   <sheetViews>
@@ -3019,511 +4260,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BC882D3-3A74-104E-AD7A-9ACBA6AE09B6}">
-  <dimension ref="A1:K22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="10">
-        <v>38</v>
-      </c>
-      <c r="C2" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D2" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E2" s="1">
-        <v>115</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="13">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="2">
-        <v>2380000</v>
-      </c>
-      <c r="K2" s="2">
-        <v>56000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="10">
-        <v>38</v>
-      </c>
-      <c r="C3" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D3" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E3" s="1">
-        <v>115</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2">
-        <v>2630000</v>
-      </c>
-      <c r="K3" s="7">
-        <v>59000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="10">
-        <v>38</v>
-      </c>
-      <c r="C4" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D4" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E4" s="1">
-        <v>115</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2">
-        <v>2750000</v>
-      </c>
-      <c r="K4" s="7">
-        <v>57000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="10">
-        <v>38</v>
-      </c>
-      <c r="C5" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D5" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E5" s="1">
-        <v>135</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="13">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2">
-        <v>33000</v>
-      </c>
-      <c r="K5" s="7">
-        <v>55000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="10">
-        <v>38</v>
-      </c>
-      <c r="C6" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D6" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E6" s="1">
-        <v>145</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="13">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2">
-        <v>73000</v>
-      </c>
-      <c r="K6" s="7">
-        <v>54000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="10">
-        <v>38</v>
-      </c>
-      <c r="C7" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D7" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E7" s="1">
-        <v>135</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2">
-        <v>34000</v>
-      </c>
-      <c r="K7" s="7">
-        <v>60000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="10">
-        <v>38</v>
-      </c>
-      <c r="C8" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D8" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E8" s="1">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="13">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="2">
-        <v>6920000</v>
-      </c>
-      <c r="K8" s="7">
-        <v>69000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="10">
-        <v>38</v>
-      </c>
-      <c r="C9" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D9" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E9" s="1">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="13">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="2">
-        <v>7590000</v>
-      </c>
-      <c r="K9" s="7">
-        <v>31000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="10">
-        <v>38</v>
-      </c>
-      <c r="C10" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D10" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E10" s="1">
-        <v>155</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="13">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="2">
-        <v>59000</v>
-      </c>
-      <c r="K10" s="7">
-        <v>56000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="7"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="7"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1377A66-7F29-A649-8A24-0084E41BD032}">
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+      <selection activeCell="A2" sqref="A2:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4267,375 +5009,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A252A25-C5BD-9644-90A1-8F508F9F4733}">
-  <dimension ref="A1:K18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="14">
-        <v>6300000</v>
-      </c>
-      <c r="K2" s="14">
-        <v>1100000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="14">
-        <v>27600000</v>
-      </c>
-      <c r="K3" s="14">
-        <v>2100000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="14">
-        <v>35700000</v>
-      </c>
-      <c r="K4" s="14">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="14">
-        <v>2300000</v>
-      </c>
-      <c r="K5" s="14">
-        <v>1300000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="14">
-        <v>313000000</v>
-      </c>
-      <c r="K6" s="14">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="14">
-        <v>37300000</v>
-      </c>
-      <c r="K7" s="14">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="14">
-        <v>1270000</v>
-      </c>
-      <c r="K8" s="14">
-        <v>1300000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="14">
-        <v>27100000</v>
-      </c>
-      <c r="K9" s="14">
-        <v>1800000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="14">
-        <v>55100000</v>
-      </c>
-      <c r="K10" s="14">
-        <v>2700000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="14">
-        <v>17700000</v>
-      </c>
-      <c r="K11" s="14">
-        <v>950000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="14">
-        <v>9100000</v>
-      </c>
-      <c r="K12" s="14">
-        <v>1300000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="14">
-        <v>2400000</v>
-      </c>
-      <c r="K13" s="14">
-        <v>1100000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="14">
-        <v>6200000</v>
-      </c>
-      <c r="K14" s="14">
-        <v>1400000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="14">
-        <v>53600000</v>
-      </c>
-      <c r="K15" s="14">
-        <v>2600000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="14">
-        <v>19900000</v>
-      </c>
-      <c r="K16" s="14">
-        <v>1700000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="14">
-        <v>45700000</v>
-      </c>
-      <c r="K17" s="14">
-        <v>2300000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="14">
-        <v>118000000</v>
-      </c>
-      <c r="K18" s="14">
-        <v>4700000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
saving figures as various file types
</commit_message>
<xml_diff>
--- a/src/text_files_for_read/Inputs.xlsx
+++ b/src/text_files_for_read/Inputs.xlsx
@@ -8,59 +8,59 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/text_files_for_read/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F998443-FD33-7B4F-BE80-2D8C682B5B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E599178-1960-F846-B7E6-A8A0F4B7182C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18260" windowHeight="16680" activeTab="1" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="1240" yWindow="460" windowWidth="24420" windowHeight="16680" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
-    <sheet name="Libarkin" sheetId="11" r:id="rId2"/>
-    <sheet name="SPICE" sheetId="9" r:id="rId3"/>
-    <sheet name="Figure 2" sheetId="10" r:id="rId4"/>
-    <sheet name="Figure 1" sheetId="8" r:id="rId5"/>
-    <sheet name="Figure 3" sheetId="7" r:id="rId6"/>
-    <sheet name="Figure 6" sheetId="5" r:id="rId7"/>
+    <sheet name="Figure 1" sheetId="8" r:id="rId2"/>
+    <sheet name="Figure 2" sheetId="10" r:id="rId3"/>
+    <sheet name="Figure 3" sheetId="7" r:id="rId4"/>
+    <sheet name="Figure 6" sheetId="5" r:id="rId5"/>
+    <sheet name="Libarkin" sheetId="11" r:id="rId6"/>
+    <sheet name="SPICE" sheetId="9" r:id="rId7"/>
     <sheet name="Sinclair" sheetId="3" r:id="rId8"/>
     <sheet name="Evenstar" sheetId="2" r:id="rId9"/>
     <sheet name="README" sheetId="4" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Active!$B$74,Active!$B$79,Active!$B$81,Active!$B$82</definedName>
-    <definedName name="solver_adj" localSheetId="5" hidden="1">'Figure 3'!$B$74,'Figure 3'!$B$79,'Figure 3'!$B$81,'Figure 3'!$B$82</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'Figure 3'!$B$74,'Figure 3'!$B$79,'Figure 3'!$B$81,'Figure 3'!$B$82</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Active!$B$85</definedName>
-    <definedName name="solver_lhs1" localSheetId="5" hidden="1">'Figure 3'!$B$85</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Figure 3'!$B$85</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Active!$F$52</definedName>
-    <definedName name="solver_lhs2" localSheetId="5" hidden="1">'Figure 3'!$F$52</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'Figure 3'!$F$52</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Active!$F$53</definedName>
-    <definedName name="solver_lhs3" localSheetId="5" hidden="1">'Figure 3'!$F$53</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'Figure 3'!$F$53</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_lin" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_num" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Active!$F$51</definedName>
-    <definedName name="solver_opt" localSheetId="5" hidden="1">'Figure 3'!$F$51</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">'Figure 3'!$F$51</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel1" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel3" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_rhs1" localSheetId="5" hidden="1">100</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0.4</definedName>
-    <definedName name="solver_rhs2" localSheetId="5" hidden="1">0.4</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">0.4</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">1.4</definedName>
-    <definedName name="solver_rhs3" localSheetId="5" hidden="1">1.4</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">1.4</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_typ" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">98.2</definedName>
-    <definedName name="solver_val" localSheetId="5" hidden="1">98.2</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">98.2</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_ver" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="82">
   <si>
     <t>Sample Name</t>
   </si>
@@ -289,9 +289,6 @@
     <t>Africa</t>
   </si>
   <si>
-    <t>EC</t>
-  </si>
-  <si>
     <t>21-11</t>
   </si>
   <si>
@@ -329,6 +326,9 @@
   </si>
   <si>
     <t>10SPC01</t>
+  </si>
+  <si>
+    <t>IN</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -476,9 +476,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -796,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39602BD4-AF2D-864A-8905-789D980EB8BD}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -848,398 +845,117 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="10">
-        <v>38</v>
-      </c>
-      <c r="C2" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D2" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E2" s="1">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="13">
-        <f>10^-6</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="2">
-        <v>2380000</v>
-      </c>
-      <c r="K2" s="2">
-        <v>56000</v>
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="9">
+        <v>20</v>
+      </c>
+      <c r="C2" s="9">
+        <v>73</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="10">
-        <v>38</v>
-      </c>
-      <c r="C3" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D3" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E3" s="1">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13">
-        <f t="shared" ref="H3:H8" si="0">10^-6</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="13"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="2">
-        <v>2630000</v>
-      </c>
-      <c r="K3" s="7">
-        <v>59000</v>
-      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="10">
-        <v>38</v>
-      </c>
-      <c r="C4" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D4" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E4" s="1">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="13"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="2">
-        <v>2750000</v>
-      </c>
-      <c r="K4" s="7">
-        <v>57000</v>
-      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="10">
-        <v>38</v>
-      </c>
-      <c r="C5" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D5" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="13"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="2">
-        <v>33000</v>
-      </c>
-      <c r="K5" s="7">
-        <v>55000</v>
-      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="10">
-        <v>38</v>
-      </c>
-      <c r="C6" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D6" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E6" s="1">
-        <v>4</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2">
-        <v>73000</v>
-      </c>
-      <c r="K6" s="7">
-        <v>54000</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="10">
-        <v>38</v>
-      </c>
-      <c r="C7" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D7" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2">
-        <v>34000</v>
-      </c>
-      <c r="K7" s="7">
-        <v>60000</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="10">
-        <v>38</v>
-      </c>
-      <c r="C8" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D8" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E8" s="1">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="2">
-        <v>59000</v>
-      </c>
-      <c r="K8" s="7">
-        <v>56000</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
+      <c r="A10" s="1"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="7"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
@@ -1327,7 +1043,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1692,11 +1408,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24694F2A-853A-E44C-A507-6368D3EEDD55}">
-  <dimension ref="A1:K10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0692F123-E8ED-A84F-B1D6-10660BCC4234}">
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1735,570 +1451,315 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="10">
-        <v>38</v>
-      </c>
-      <c r="C2" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D2" s="10">
-        <v>2500</v>
+        <v>12</v>
+      </c>
+      <c r="B2" s="9">
+        <v>90</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
       </c>
       <c r="H2" s="13">
-        <f>10^-6</f>
-        <v>9.9999999999999995E-7</v>
+        <v>0</v>
       </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="2">
-        <v>2380000</v>
-      </c>
-      <c r="K2" s="2">
-        <v>56000</v>
+      <c r="J2" s="1">
+        <f>65.91*10^7</f>
+        <v>659100000</v>
+      </c>
+      <c r="K2" s="1">
+        <f>1.2*10^7</f>
+        <v>12000000</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="B3" s="10">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="C3" s="10">
-        <v>-106</v>
+        <v>0</v>
       </c>
       <c r="D3" s="10">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
       <c r="H3" s="13">
-        <f t="shared" ref="H3:H8" si="0">10^-6</f>
-        <v>9.9999999999999995E-7</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="2">
-        <v>2630000</v>
-      </c>
-      <c r="K3" s="7">
-        <v>59000</v>
+        <f>74.48*10^7</f>
+        <v>744800000</v>
+      </c>
+      <c r="K3" s="2">
+        <f>2.33*10^7</f>
+        <v>23300000</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>61</v>
+      <c r="A4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B4" s="10">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="C4" s="10">
-        <v>-106</v>
+        <v>0</v>
       </c>
       <c r="D4" s="10">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="E4" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
       </c>
       <c r="H4" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
+        <v>0</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="2">
-        <v>2750000</v>
-      </c>
-      <c r="K4" s="7">
-        <v>57000</v>
+        <f>91.1*10^7</f>
+        <v>911000000</v>
+      </c>
+      <c r="K4" s="2">
+        <f>1.3*10^7</f>
+        <v>13000000</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>59</v>
+      <c r="A5" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B5" s="10">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="C5" s="10">
-        <v>-106</v>
+        <v>0</v>
       </c>
       <c r="D5" s="10">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="E5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
       </c>
       <c r="H5" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="2">
-        <v>33000</v>
-      </c>
-      <c r="K5" s="7">
-        <v>55000</v>
+        <f>167.12*10^7</f>
+        <v>1671200000</v>
+      </c>
+      <c r="K5" s="2">
+        <f>3.65*10^7</f>
+        <v>36500000</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="10">
-        <v>38</v>
-      </c>
-      <c r="C6" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D6" s="10">
-        <v>2500</v>
+      <c r="A6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="9">
+        <v>90</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2000</v>
       </c>
       <c r="E6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
       </c>
       <c r="H6" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2">
-        <v>73000</v>
-      </c>
-      <c r="K6" s="7">
-        <v>54000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>63</v>
+      <c r="A7" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="B7" s="10">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="C7" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D7" s="10">
-        <v>2500</v>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2000</v>
       </c>
       <c r="E7" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
       </c>
       <c r="H7" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2">
-        <v>34000</v>
-      </c>
-      <c r="K7" s="7">
-        <v>60000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>60</v>
+      <c r="A8" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="B8" s="10">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="C8" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D8" s="10">
-        <v>2500</v>
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4000</v>
       </c>
       <c r="E8" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F8" s="1">
-        <v>2.3199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
       </c>
       <c r="H8" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="2">
-        <v>59000</v>
-      </c>
-      <c r="K8" s="7">
-        <v>56000</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4000</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="16"/>
+      <c r="A10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="9">
+        <v>90</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D985B3A1-D71F-474D-89CB-3BE7E854D433}">
-  <dimension ref="A1:K9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="15">
-        <v>35.5944</v>
-      </c>
-      <c r="C2" s="15">
-        <v>111.63420000000001</v>
-      </c>
-      <c r="D2" s="15">
-        <v>1837</v>
-      </c>
-      <c r="E2" s="15">
-        <v>8</v>
-      </c>
-      <c r="F2" s="15">
-        <v>2.25</v>
-      </c>
-      <c r="G2" s="15">
-        <v>0.99</v>
-      </c>
-      <c r="H2" s="15">
-        <v>0</v>
-      </c>
-      <c r="J2" s="15">
-        <f>4.09*10^6</f>
-        <v>4090000</v>
-      </c>
-      <c r="K2">
-        <f>0.45*10^6</f>
-        <v>450000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="15">
-        <v>35.605600000000003</v>
-      </c>
-      <c r="C3" s="15">
-        <v>111.61750000000001</v>
-      </c>
-      <c r="D3" s="15">
-        <v>1807</v>
-      </c>
-      <c r="E3" s="15">
-        <v>8</v>
-      </c>
-      <c r="F3" s="15">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="G3" s="15">
-        <v>0.99</v>
-      </c>
-      <c r="H3" s="15">
-        <v>0</v>
-      </c>
-      <c r="J3" s="15">
-        <f>4.42*10^6</f>
-        <v>4420000</v>
-      </c>
-      <c r="K3">
-        <f>0.44*10^6</f>
-        <v>440000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="15">
-        <v>35.61</v>
-      </c>
-      <c r="C4" s="15">
-        <v>111.61369999999999</v>
-      </c>
-      <c r="D4" s="15">
-        <v>1810</v>
-      </c>
-      <c r="E4" s="15">
-        <v>13</v>
-      </c>
-      <c r="F4" s="15">
-        <v>3.15</v>
-      </c>
-      <c r="G4" s="15">
-        <v>0.99</v>
-      </c>
-      <c r="H4" s="15">
-        <v>0</v>
-      </c>
-      <c r="J4" s="15">
-        <f>4.17*10^6</f>
-        <v>4170000</v>
-      </c>
-      <c r="K4">
-        <f>0.39*10^6</f>
-        <v>390000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="15">
-        <v>35.616300000000003</v>
-      </c>
-      <c r="C5" s="15">
-        <v>111.60809999999999</v>
-      </c>
-      <c r="D5" s="15">
-        <v>1800</v>
-      </c>
-      <c r="E5" s="15">
-        <v>13</v>
-      </c>
-      <c r="F5" s="15">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="G5" s="15">
-        <v>1</v>
-      </c>
-      <c r="H5" s="15">
-        <v>0</v>
-      </c>
-      <c r="J5" s="15">
-        <f>4.16*10^6</f>
-        <v>4160000</v>
-      </c>
-      <c r="K5">
-        <f>0.46*10^6</f>
-        <v>460000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="15">
-        <v>35.624499999999998</v>
-      </c>
-      <c r="C6" s="15">
-        <v>111.6057</v>
-      </c>
-      <c r="D6" s="15">
-        <v>1778</v>
-      </c>
-      <c r="E6" s="15">
-        <v>13</v>
-      </c>
-      <c r="F6" s="15">
-        <v>2.29</v>
-      </c>
-      <c r="G6" s="15">
-        <v>1</v>
-      </c>
-      <c r="H6" s="15">
-        <v>0</v>
-      </c>
-      <c r="J6" s="15">
-        <f>3.9*10^6</f>
-        <v>3900000</v>
-      </c>
-      <c r="K6">
-        <f>0.45*10^6</f>
-        <v>450000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="15">
-        <v>35.616399999999999</v>
-      </c>
-      <c r="C7" s="15">
-        <v>111.6087</v>
-      </c>
-      <c r="D7" s="15">
-        <v>1800</v>
-      </c>
-      <c r="E7" s="15">
-        <v>13</v>
-      </c>
-      <c r="F7" s="15">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="G7" s="15">
-        <v>1</v>
-      </c>
-      <c r="H7" s="15">
-        <v>0</v>
-      </c>
-      <c r="J7" s="15">
-        <f>4.02*10^6</f>
-        <v>4019999.9999999995</v>
-      </c>
-      <c r="K7">
-        <f>0.52*10^6</f>
-        <v>520000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="15">
-        <v>35.609400000000001</v>
-      </c>
-      <c r="C8" s="15">
-        <v>111.6135</v>
-      </c>
-      <c r="D8" s="15">
-        <v>1810</v>
-      </c>
-      <c r="E8" s="15">
-        <v>13</v>
-      </c>
-      <c r="F8" s="15">
-        <v>2.29</v>
-      </c>
-      <c r="G8" s="15">
-        <v>0.99</v>
-      </c>
-      <c r="H8" s="15">
-        <v>0</v>
-      </c>
-      <c r="J8" s="15">
-        <f>4.17*10^6</f>
-        <v>4170000</v>
-      </c>
-      <c r="K8">
-        <f>0.66*10^6</f>
-        <v>660000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="15">
-        <v>35.587800000000001</v>
-      </c>
-      <c r="C9" s="15">
-        <v>111.6345</v>
-      </c>
-      <c r="D9" s="15">
-        <v>1876</v>
-      </c>
-      <c r="E9" s="15">
-        <v>6</v>
-      </c>
-      <c r="F9" s="15">
-        <v>2.25</v>
-      </c>
-      <c r="G9" s="15">
-        <v>0.99</v>
-      </c>
-      <c r="H9" s="15">
-        <v>0</v>
-      </c>
-      <c r="J9" s="15">
-        <f>4.36*10^6</f>
-        <v>4360000</v>
-      </c>
-      <c r="K9">
-        <f>0.47*10^6</f>
-        <v>470000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345E843F-B5AF-7544-9892-CA1AD39C5E9D}">
   <dimension ref="A1:K20"/>
   <sheetViews>
@@ -2554,364 +2015,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0692F123-E8ED-A84F-B1D6-10660BCC4234}">
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="9">
-        <v>90</v>
-      </c>
-      <c r="C2" s="9">
-        <v>0</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="13">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1">
-        <f>65.91*10^7</f>
-        <v>659100000</v>
-      </c>
-      <c r="K2" s="1">
-        <f>1.2*10^7</f>
-        <v>12000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10">
-        <v>0</v>
-      </c>
-      <c r="C3" s="10">
-        <v>0</v>
-      </c>
-      <c r="D3" s="10">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2">
-        <f>74.48*10^7</f>
-        <v>744800000</v>
-      </c>
-      <c r="K3" s="2">
-        <f>2.33*10^7</f>
-        <v>23300000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="10">
-        <v>90</v>
-      </c>
-      <c r="C4" s="10">
-        <v>0</v>
-      </c>
-      <c r="D4" s="10">
-        <v>1000</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2">
-        <f>91.1*10^7</f>
-        <v>911000000</v>
-      </c>
-      <c r="K4" s="2">
-        <f>1.3*10^7</f>
-        <v>13000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="10">
-        <v>0</v>
-      </c>
-      <c r="C5" s="10">
-        <v>0</v>
-      </c>
-      <c r="D5" s="10">
-        <v>1000</v>
-      </c>
-      <c r="E5" s="1">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="13">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2">
-        <f>167.12*10^7</f>
-        <v>1671200000</v>
-      </c>
-      <c r="K5" s="2">
-        <f>3.65*10^7</f>
-        <v>36500000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="9">
-        <v>90</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2000</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="10">
-        <v>0</v>
-      </c>
-      <c r="C7" s="10">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2000</v>
-      </c>
-      <c r="E7" s="1">
-        <v>5</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="10">
-        <v>90</v>
-      </c>
-      <c r="C8" s="10">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E8" s="1">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="10">
-        <v>0</v>
-      </c>
-      <c r="C9" s="10">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="9">
-        <v>90</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>6000</v>
-      </c>
-      <c r="E10" s="1">
-        <v>5</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="10">
-        <v>0</v>
-      </c>
-      <c r="C11" s="10">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>6000</v>
-      </c>
-      <c r="E11" s="1">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2CA47B-538E-684E-879A-957351F4517A}">
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3332,12 +2441,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9FD288-F7FF-CC43-984C-6BC5F64D5A7D}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD11"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3376,142 +2485,668 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="B2" s="9">
+        <v>20</v>
+      </c>
+      <c r="C2" s="9">
+        <v>73</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24694F2A-853A-E44C-A507-6368D3EEDD55}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="10">
+        <v>38</v>
+      </c>
+      <c r="C2" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <f>10^-6</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2">
+        <v>2380000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>56000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="10">
+        <v>38</v>
+      </c>
+      <c r="C3" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D3" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <f t="shared" ref="H3:H8" si="0">10^-6</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2">
+        <v>2630000</v>
+      </c>
+      <c r="K3" s="7">
+        <v>59000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="10">
+        <v>38</v>
+      </c>
+      <c r="C4" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D4" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2">
+        <v>2750000</v>
+      </c>
+      <c r="K4" s="7">
+        <v>57000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="10">
+        <v>38</v>
+      </c>
+      <c r="C5" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2">
+        <v>33000</v>
+      </c>
+      <c r="K5" s="7">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="10">
+        <v>38</v>
+      </c>
+      <c r="C6" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2">
+        <v>73000</v>
+      </c>
+      <c r="K6" s="7">
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="10">
+        <v>38</v>
+      </c>
+      <c r="C7" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D7" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2">
+        <v>34000</v>
+      </c>
+      <c r="K7" s="7">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="10">
+        <v>38</v>
+      </c>
+      <c r="C8" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2">
+        <v>59000</v>
+      </c>
+      <c r="K8" s="7">
+        <v>56000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D985B3A1-D71F-474D-89CB-3BE7E854D433}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="15">
+        <v>35.5944</v>
+      </c>
+      <c r="C2" s="15">
+        <v>111.63420000000001</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1837</v>
+      </c>
+      <c r="E2" s="15">
+        <v>8</v>
+      </c>
+      <c r="F2" s="15">
+        <v>2.25</v>
+      </c>
+      <c r="G2" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0</v>
+      </c>
+      <c r="J2" s="15">
+        <f>4.09*10^6</f>
+        <v>4090000</v>
+      </c>
+      <c r="K2">
+        <f>0.45*10^6</f>
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="15">
+        <v>35.605600000000003</v>
+      </c>
+      <c r="C3" s="15">
+        <v>111.61750000000001</v>
+      </c>
+      <c r="D3" s="15">
+        <v>1807</v>
+      </c>
+      <c r="E3" s="15">
+        <v>8</v>
+      </c>
+      <c r="F3" s="15">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="G3" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="H3" s="15">
+        <v>0</v>
+      </c>
+      <c r="J3" s="15">
+        <f>4.42*10^6</f>
+        <v>4420000</v>
+      </c>
+      <c r="K3">
+        <f>0.44*10^6</f>
+        <v>440000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="9">
-        <v>-42</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="9">
-        <v>75</v>
-      </c>
-      <c r="C3" s="9">
-        <v>-42</v>
-      </c>
-      <c r="D3" s="9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="9">
-        <v>75</v>
-      </c>
-      <c r="C4" s="9">
-        <v>-42</v>
-      </c>
-      <c r="D4" s="9">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="15">
+        <v>35.61</v>
+      </c>
+      <c r="C4" s="15">
+        <v>111.61369999999999</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1810</v>
+      </c>
+      <c r="E4" s="15">
+        <v>13</v>
+      </c>
+      <c r="F4" s="15">
+        <v>3.15</v>
+      </c>
+      <c r="G4" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="H4" s="15">
+        <v>0</v>
+      </c>
+      <c r="J4" s="15">
+        <f>4.17*10^6</f>
+        <v>4170000</v>
+      </c>
+      <c r="K4">
+        <f>0.39*10^6</f>
+        <v>390000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="9">
-        <v>75</v>
-      </c>
-      <c r="C5" s="9">
-        <v>-42</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="B5" s="15">
+        <v>35.616300000000003</v>
+      </c>
+      <c r="C5" s="15">
+        <v>111.60809999999999</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1800</v>
+      </c>
+      <c r="E5" s="15">
+        <v>13</v>
+      </c>
+      <c r="F5" s="15">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="G5" s="15">
+        <v>1</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0</v>
+      </c>
+      <c r="J5" s="15">
+        <f>4.16*10^6</f>
+        <v>4160000</v>
+      </c>
+      <c r="K5">
+        <f>0.46*10^6</f>
+        <v>460000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="9">
-        <v>75</v>
-      </c>
-      <c r="C6" s="9">
-        <v>-42</v>
-      </c>
-      <c r="D6" s="9">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="B6" s="15">
+        <v>35.624499999999998</v>
+      </c>
+      <c r="C6" s="15">
+        <v>111.6057</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1778</v>
+      </c>
+      <c r="E6" s="15">
+        <v>13</v>
+      </c>
+      <c r="F6" s="15">
+        <v>2.29</v>
+      </c>
+      <c r="G6" s="15">
+        <v>1</v>
+      </c>
+      <c r="H6" s="15">
+        <v>0</v>
+      </c>
+      <c r="J6" s="15">
+        <f>3.9*10^6</f>
+        <v>3900000</v>
+      </c>
+      <c r="K6">
+        <f>0.45*10^6</f>
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0</v>
-      </c>
-      <c r="C7" s="9">
-        <v>-78</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="B7" s="15">
+        <v>35.616399999999999</v>
+      </c>
+      <c r="C7" s="15">
+        <v>111.6087</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1800</v>
+      </c>
+      <c r="E7" s="15">
+        <v>13</v>
+      </c>
+      <c r="F7" s="15">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="G7" s="15">
+        <v>1</v>
+      </c>
+      <c r="H7" s="15">
+        <v>0</v>
+      </c>
+      <c r="J7" s="15">
+        <f>4.02*10^6</f>
+        <v>4019999.9999999995</v>
+      </c>
+      <c r="K7">
+        <f>0.52*10^6</f>
+        <v>520000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="9">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9">
-        <v>-78</v>
-      </c>
-      <c r="D8" s="9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="B8" s="15">
+        <v>35.609400000000001</v>
+      </c>
+      <c r="C8" s="15">
+        <v>111.6135</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1810</v>
+      </c>
+      <c r="E8" s="15">
+        <v>13</v>
+      </c>
+      <c r="F8" s="15">
+        <v>2.29</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="H8" s="15">
+        <v>0</v>
+      </c>
+      <c r="J8" s="15">
+        <f>4.17*10^6</f>
+        <v>4170000</v>
+      </c>
+      <c r="K8">
+        <f>0.66*10^6</f>
+        <v>660000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="9">
-        <v>0</v>
-      </c>
-      <c r="C9" s="9">
-        <v>-78</v>
-      </c>
-      <c r="D9" s="9">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0</v>
-      </c>
-      <c r="C10" s="9">
-        <v>-78</v>
-      </c>
-      <c r="D10" s="9">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="9">
-        <v>0</v>
-      </c>
-      <c r="C11" s="9">
-        <v>-78</v>
-      </c>
-      <c r="D11" s="9">
-        <v>5000</v>
+        <v>80</v>
+      </c>
+      <c r="B9" s="15">
+        <v>35.587800000000001</v>
+      </c>
+      <c r="C9" s="15">
+        <v>111.6345</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1876</v>
+      </c>
+      <c r="E9" s="15">
+        <v>6</v>
+      </c>
+      <c r="F9" s="15">
+        <v>2.25</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="J9" s="15">
+        <f>4.36*10^6</f>
+        <v>4360000</v>
+      </c>
+      <c r="K9">
+        <f>0.47*10^6</f>
+        <v>470000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed libarkin dataset plot
</commit_message>
<xml_diff>
--- a/src/text_files_for_read/Inputs.xlsx
+++ b/src/text_files_for_read/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/text_files_for_read/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E599178-1960-F846-B7E6-A8A0F4B7182C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E676FE7E-124A-9B4D-B71F-5880CC7E6518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="460" windowWidth="24420" windowHeight="16680" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="82">
   <si>
     <t>Sample Name</t>
   </si>
@@ -794,7 +794,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,87 +845,242 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="9">
-        <v>20</v>
-      </c>
-      <c r="C2" s="9">
-        <v>73</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0</v>
+      <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="10">
+        <v>38</v>
+      </c>
+      <c r="C2" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <f>10^-6</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="2">
+        <v>2380000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>56000</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="13"/>
+      <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="10">
+        <v>38</v>
+      </c>
+      <c r="C3" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D3" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <f t="shared" ref="H3:H8" si="0">10^-6</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="J3" s="2">
+        <v>2630000</v>
+      </c>
+      <c r="K3" s="7">
+        <v>59000</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="13"/>
+      <c r="A4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="10">
+        <v>38</v>
+      </c>
+      <c r="C4" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D4" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="J4" s="2">
+        <v>2750000</v>
+      </c>
+      <c r="K4" s="7">
+        <v>57000</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="13"/>
+      <c r="A5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="10">
+        <v>38</v>
+      </c>
+      <c r="C5" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="J5" s="2">
+        <v>330000</v>
+      </c>
+      <c r="K5" s="7">
+        <v>550000</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="13"/>
+      <c r="A6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="10">
+        <v>38</v>
+      </c>
+      <c r="C6" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2">
+        <v>730000</v>
+      </c>
+      <c r="K6" s="7">
+        <v>540000</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="13"/>
+      <c r="A7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="10">
+        <v>38</v>
+      </c>
+      <c r="C7" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D7" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2">
+        <v>340000</v>
+      </c>
+      <c r="K7" s="7">
+        <v>600000</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="13"/>
+      <c r="A8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="10">
+        <v>38</v>
+      </c>
+      <c r="C8" s="10">
+        <v>-106</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2500</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2">
+        <v>590000</v>
+      </c>
+      <c r="K8" s="7">
+        <v>560000</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -2552,7 +2707,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2719,10 +2874,10 @@
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="2">
-        <v>33000</v>
+        <v>330000</v>
       </c>
       <c r="K5" s="7">
-        <v>55000</v>
+        <v>550000</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -2753,10 +2908,10 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="2">
-        <v>73000</v>
+        <v>730000</v>
       </c>
       <c r="K6" s="7">
-        <v>54000</v>
+        <v>540000</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2787,10 +2942,10 @@
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="2">
-        <v>34000</v>
+        <v>340000</v>
       </c>
       <c r="K7" s="7">
-        <v>60000</v>
+        <v>600000</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -2821,10 +2976,10 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="2">
-        <v>59000</v>
+        <v>590000</v>
       </c>
       <c r="K8" s="7">
-        <v>56000</v>
+        <v>560000</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added 'means' variable to updated MCADAM.py script
</commit_message>
<xml_diff>
--- a/src/text_files_for_read/Inputs.xlsx
+++ b/src/text_files_for_read/Inputs.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmijjum/Documents/Production_Rates_Calculator/src/text_files_for_read/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E676FE7E-124A-9B4D-B71F-5880CC7E6518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835EE8FB-3DF0-2843-909E-22CDEA7EEE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
+    <workbookView xWindow="80" yWindow="1380" windowWidth="28800" windowHeight="16580" xr2:uid="{908D5193-7DFE-C84B-BF15-EFFE4A8B620F}"/>
   </bookViews>
   <sheets>
     <sheet name="Active" sheetId="1" r:id="rId1"/>
     <sheet name="Figure 1" sheetId="8" r:id="rId2"/>
     <sheet name="Figure 2" sheetId="10" r:id="rId3"/>
     <sheet name="Figure 3" sheetId="7" r:id="rId4"/>
-    <sheet name="Figure 6" sheetId="5" r:id="rId5"/>
-    <sheet name="Libarkin" sheetId="11" r:id="rId6"/>
-    <sheet name="SPICE" sheetId="9" r:id="rId7"/>
-    <sheet name="Sinclair" sheetId="3" r:id="rId8"/>
-    <sheet name="Evenstar" sheetId="2" r:id="rId9"/>
-    <sheet name="README" sheetId="4" r:id="rId10"/>
+    <sheet name="Figure 5" sheetId="12" r:id="rId5"/>
+    <sheet name="Figure 6" sheetId="5" r:id="rId6"/>
+    <sheet name="Libarkin" sheetId="11" r:id="rId7"/>
+    <sheet name="SPICE" sheetId="9" r:id="rId8"/>
+    <sheet name="Sinclair" sheetId="3" r:id="rId9"/>
+    <sheet name="Evenstar" sheetId="2" r:id="rId10"/>
+    <sheet name="README" sheetId="4" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Active!$B$74,Active!$B$79,Active!$B$81,Active!$B$82</definedName>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="83">
   <si>
     <t>Sample Name</t>
   </si>
@@ -329,6 +330,9 @@
   </si>
   <si>
     <t>IN</t>
+  </si>
+  <si>
+    <t>EC</t>
   </si>
 </sst>
 </file>
@@ -433,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -476,6 +480,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -794,7 +801,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,344 +852,343 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="10">
-        <v>38</v>
-      </c>
-      <c r="C2" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D2" s="10">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>75</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>75</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>75</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6">
+        <v>75</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7">
+        <v>75</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8">
+        <v>75</v>
+      </c>
+      <c r="C8">
+        <v>40</v>
+      </c>
+      <c r="D8">
         <v>2500</v>
       </c>
-      <c r="E2" s="1">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="13">
-        <f>10^-6</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="2">
-        <v>2380000</v>
-      </c>
-      <c r="K2" s="2">
-        <v>56000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="10">
-        <v>38</v>
-      </c>
-      <c r="C3" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D3" s="10">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9">
+        <v>75</v>
+      </c>
+      <c r="C9">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10">
+        <v>75</v>
+      </c>
+      <c r="C10">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11">
+        <v>75</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>78</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>78</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>78</v>
+      </c>
+      <c r="D14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>78</v>
+      </c>
+      <c r="D15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>78</v>
+      </c>
+      <c r="D16">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>78</v>
+      </c>
+      <c r="D17">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>78</v>
+      </c>
+      <c r="D18">
         <v>2500</v>
       </c>
-      <c r="E3" s="1">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13">
-        <f t="shared" ref="H3:H8" si="0">10^-6</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2">
-        <v>2630000</v>
-      </c>
-      <c r="K3" s="7">
-        <v>59000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="10">
-        <v>38</v>
-      </c>
-      <c r="C4" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D4" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E4" s="1">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2">
-        <v>2750000</v>
-      </c>
-      <c r="K4" s="7">
-        <v>57000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="10">
-        <v>38</v>
-      </c>
-      <c r="C5" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D5" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2">
-        <v>330000</v>
-      </c>
-      <c r="K5" s="7">
-        <v>550000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="10">
-        <v>38</v>
-      </c>
-      <c r="C6" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D6" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E6" s="1">
-        <v>4</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2">
-        <v>730000</v>
-      </c>
-      <c r="K6" s="7">
-        <v>540000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="10">
-        <v>38</v>
-      </c>
-      <c r="C7" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D7" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2">
-        <v>340000</v>
-      </c>
-      <c r="K7" s="7">
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="10">
-        <v>38</v>
-      </c>
-      <c r="C8" s="10">
-        <v>-106</v>
-      </c>
-      <c r="D8" s="10">
-        <v>2500</v>
-      </c>
-      <c r="E8" s="1">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="2">
-        <v>590000</v>
-      </c>
-      <c r="K8" s="7">
-        <v>560000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="7"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>78</v>
+      </c>
+      <c r="D19">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>78</v>
+      </c>
+      <c r="D20">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>78</v>
+      </c>
+      <c r="D21">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22" s="10"/>
       <c r="E22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B23" s="10"/>
       <c r="E23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B24" s="10"/>
       <c r="E24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B25" s="9"/>
       <c r="E25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26" s="9"/>
       <c r="E26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B27" s="9"/>
       <c r="E27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28" s="9"/>
       <c r="E28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -1194,6 +1200,757 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1377A66-7F29-A649-8A24-0084E41BD032}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9">
+        <v>-19.578942000000001</v>
+      </c>
+      <c r="C2" s="9">
+        <v>-69.872967000000003</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1172</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1">
+        <f>65.91*10^7</f>
+        <v>659100000</v>
+      </c>
+      <c r="K2" s="1">
+        <f>1.2*10^7</f>
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="10">
+        <v>-19.340944</v>
+      </c>
+      <c r="C3" s="10">
+        <v>-69.727999999999994</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1607</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2">
+        <f>74.48*10^7</f>
+        <v>744800000</v>
+      </c>
+      <c r="K3" s="2">
+        <f>2.33*10^7</f>
+        <v>23300000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="10">
+        <v>-19.340944</v>
+      </c>
+      <c r="C4" s="10">
+        <v>-69.727999999999994</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1607</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="2">
+        <f>91.1*10^7</f>
+        <v>911000000</v>
+      </c>
+      <c r="K4" s="2">
+        <f>1.3*10^7</f>
+        <v>13000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="10">
+        <v>-19.340944</v>
+      </c>
+      <c r="C5" s="10">
+        <v>-69.727999999999994</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1607</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2">
+        <f>167.12*10^7</f>
+        <v>1671200000</v>
+      </c>
+      <c r="K5" s="2">
+        <f>3.65*10^7</f>
+        <v>36500000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10">
+        <v>-19.336722000000002</v>
+      </c>
+      <c r="C6" s="10">
+        <v>-69.729611000000006</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1604</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2">
+        <f>104.68*10^7</f>
+        <v>1046800000.0000001</v>
+      </c>
+      <c r="K6" s="2">
+        <f>2.24*10^7</f>
+        <v>22400000.000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="9">
+        <v>-18.886583000000002</v>
+      </c>
+      <c r="C7" s="9">
+        <v>-69.699055999999999</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2282</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2">
+        <f>269.89*10^7</f>
+        <v>2698900000</v>
+      </c>
+      <c r="K7" s="7">
+        <f>4.73*10^7</f>
+        <v>47300000.000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="9">
+        <v>-18.886583000000002</v>
+      </c>
+      <c r="C8" s="9">
+        <v>-69.699055999999999</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2282</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2">
+        <f>246.53*10^7</f>
+        <v>2465300000</v>
+      </c>
+      <c r="K8" s="7">
+        <f>4.29*10^7</f>
+        <v>42900000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="9">
+        <v>-18.905639000000001</v>
+      </c>
+      <c r="C9" s="9">
+        <v>-69.954583</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1443</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="2">
+        <f>141.41*10^7</f>
+        <v>1414100000</v>
+      </c>
+      <c r="K9" s="7">
+        <f>2.52*10^7</f>
+        <v>25200000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="9">
+        <v>-18.905639000000001</v>
+      </c>
+      <c r="C10" s="9">
+        <v>-69.954583</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1443</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="2">
+        <f>164.8*10^7</f>
+        <v>1648000000</v>
+      </c>
+      <c r="K10" s="7">
+        <f>2.84*10^7</f>
+        <v>28400000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="9">
+        <v>-18.852694</v>
+      </c>
+      <c r="C11" s="9">
+        <v>-69.657167000000001</v>
+      </c>
+      <c r="D11" s="9">
+        <v>2550</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="2">
+        <f>235*10^7</f>
+        <v>2350000000</v>
+      </c>
+      <c r="K11" s="7">
+        <f>4.04*10^7</f>
+        <v>40400000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9">
+        <v>-20.704083000000001</v>
+      </c>
+      <c r="C12" s="9">
+        <v>-69.420833000000002</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1084</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="13">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="2">
+        <f>90.19*10^7</f>
+        <v>901900000</v>
+      </c>
+      <c r="K12" s="7">
+        <f>1.97*10^7</f>
+        <v>19700000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="11">
+        <v>-19.786306</v>
+      </c>
+      <c r="C13" s="11">
+        <v>-69.682000000000002</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1289</v>
+      </c>
+      <c r="E13" s="1">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="2">
+        <f>107.8*10^7</f>
+        <v>1078000000</v>
+      </c>
+      <c r="K13" s="2">
+        <f>2.77*10^7</f>
+        <v>27700000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="10">
+        <v>-19.786306</v>
+      </c>
+      <c r="C14" s="10">
+        <v>-69.682000000000002</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1289</v>
+      </c>
+      <c r="E14" s="1">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="2">
+        <f>102.49*10^7</f>
+        <v>1024900000</v>
+      </c>
+      <c r="K14" s="2">
+        <f>2.48*10^7</f>
+        <v>24800000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="10">
+        <v>-19.786306</v>
+      </c>
+      <c r="C15" s="10">
+        <v>-69.682000000000002</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1289</v>
+      </c>
+      <c r="E15" s="1">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="13">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="8">
+        <f>298.96*10^7</f>
+        <v>2989600000</v>
+      </c>
+      <c r="K15" s="2">
+        <f>3.2*10^7</f>
+        <v>32000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="10">
+        <v>-19.397832999999999</v>
+      </c>
+      <c r="C16" s="10">
+        <v>-69.880306000000004</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1256</v>
+      </c>
+      <c r="E16" s="1">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="13">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="2">
+        <f>194.23*10^7</f>
+        <v>1942300000</v>
+      </c>
+      <c r="K16" s="2">
+        <f>4.67*10^7</f>
+        <v>46700000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="10">
+        <v>-19.397832999999999</v>
+      </c>
+      <c r="C17" s="10">
+        <v>-69.880306000000004</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1256</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2.74</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="13">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="2">
+        <f>310.26*10^7</f>
+        <v>3102600000</v>
+      </c>
+      <c r="K17" s="2">
+        <f>8.23*10^7</f>
+        <v>82300000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="10">
+        <v>-19.397832999999999</v>
+      </c>
+      <c r="C18" s="10">
+        <v>-69.880306000000004</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1256</v>
+      </c>
+      <c r="E18" s="1">
+        <v>5</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="13">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="2">
+        <f>269.16*10^7</f>
+        <v>2691600000.0000005</v>
+      </c>
+      <c r="K18" s="2">
+        <f>6.18*10^7</f>
+        <v>61800000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="9">
+        <v>-19.522110999999999</v>
+      </c>
+      <c r="C19" s="9">
+        <v>-69.808333000000005</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1312</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="13">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="2">
+        <f>277.15*10^7</f>
+        <v>2771500000</v>
+      </c>
+      <c r="K19" s="7">
+        <f>5.2*10^7</f>
+        <v>52000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="9">
+        <v>-19.522110999999999</v>
+      </c>
+      <c r="C20" s="9">
+        <v>-69.808333000000005</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1312</v>
+      </c>
+      <c r="E20" s="1">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="13">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="2">
+        <f>65.4*10^7</f>
+        <v>654000000</v>
+      </c>
+      <c r="K20" s="7">
+        <f>1.5*10^7</f>
+        <v>15000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="12">
+        <v>-18.503527999999999</v>
+      </c>
+      <c r="C21" s="12">
+        <v>-70.143305999999995</v>
+      </c>
+      <c r="D21" s="12">
+        <v>771</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="13">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="2">
+        <f>41.29*10^7</f>
+        <v>412900000</v>
+      </c>
+      <c r="K21" s="7">
+        <f>0.72*10^7</f>
+        <v>7200000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A252A25-C5BD-9644-90A1-8F508F9F4733}">
   <dimension ref="A1:K18"/>
   <sheetViews>
@@ -2175,7 +2932,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2597,6 +3354,333 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923D42B9-7A86-1345-AADD-F9A6DEC8D2BA}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>75</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>75</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4">
+        <v>75</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6">
+        <v>75</v>
+      </c>
+      <c r="C6">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7">
+        <v>75</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8">
+        <v>75</v>
+      </c>
+      <c r="C8">
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9">
+        <v>75</v>
+      </c>
+      <c r="C9">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10">
+        <v>75</v>
+      </c>
+      <c r="C10">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11">
+        <v>75</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>78</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>78</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>78</v>
+      </c>
+      <c r="D14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>78</v>
+      </c>
+      <c r="D15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>78</v>
+      </c>
+      <c r="D16">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>78</v>
+      </c>
+      <c r="D17">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>78</v>
+      </c>
+      <c r="D18">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>78</v>
+      </c>
+      <c r="D19">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>78</v>
+      </c>
+      <c r="D20">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>78</v>
+      </c>
+      <c r="D21">
+        <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9FD288-F7FF-CC43-984C-6BC5F64D5A7D}">
   <dimension ref="A1:K11"/>
   <sheetViews>
@@ -2702,17 +3786,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24694F2A-853A-E44C-A507-6368D3EEDD55}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2744,7 +3828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
@@ -2766,10 +3850,7 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="13">
-        <f>10^-6</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
+      <c r="H2" s="13"/>
       <c r="I2" s="1"/>
       <c r="J2" s="2">
         <v>2380000</v>
@@ -2777,8 +3858,11 @@
       <c r="K2" s="2">
         <v>56000</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
@@ -2800,10 +3884,7 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="13">
-        <f t="shared" ref="H3:H8" si="0">10^-6</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
+      <c r="H3" s="13"/>
       <c r="I3" s="1"/>
       <c r="J3" s="2">
         <v>2630000</v>
@@ -2811,8 +3892,11 @@
       <c r="K3" s="7">
         <v>59000</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
@@ -2834,10 +3918,7 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
+      <c r="H4" s="13"/>
       <c r="I4" s="1"/>
       <c r="J4" s="2">
         <v>2750000</v>
@@ -2845,8 +3926,11 @@
       <c r="K4" s="7">
         <v>57000</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>59</v>
       </c>
@@ -2868,10 +3952,7 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
+      <c r="H5" s="13"/>
       <c r="I5" s="1"/>
       <c r="J5" s="2">
         <v>330000</v>
@@ -2879,8 +3960,11 @@
       <c r="K5" s="7">
         <v>550000</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>62</v>
       </c>
@@ -2902,10 +3986,7 @@
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
+      <c r="H6" s="13"/>
       <c r="I6" s="1"/>
       <c r="J6" s="2">
         <v>730000</v>
@@ -2913,8 +3994,11 @@
       <c r="K6" s="7">
         <v>540000</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>63</v>
       </c>
@@ -2936,10 +4020,7 @@
       <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="H7" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
+      <c r="H7" s="13"/>
       <c r="I7" s="1"/>
       <c r="J7" s="2">
         <v>340000</v>
@@ -2947,8 +4028,11 @@
       <c r="K7" s="7">
         <v>600000</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>60</v>
       </c>
@@ -2970,10 +4054,7 @@
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="13">
-        <f t="shared" si="0"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
+      <c r="H8" s="13"/>
       <c r="I8" s="1"/>
       <c r="J8" s="2">
         <v>590000</v>
@@ -2981,16 +4062,27 @@
       <c r="K8" s="7">
         <v>560000</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <v>27.5</v>
+      </c>
+      <c r="C11" s="16">
+        <v>28.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D985B3A1-D71F-474D-89CB-3BE7E854D433}">
   <dimension ref="A1:K9"/>
   <sheetViews>
@@ -3309,7 +4401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081048F5-9F92-C54B-B1C5-62D0C1F0285D}">
   <dimension ref="A1:K39"/>
   <sheetViews>
@@ -4048,755 +5140,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1377A66-7F29-A649-8A24-0084E41BD032}">
-  <dimension ref="A1:K21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="9">
-        <v>-19.578942000000001</v>
-      </c>
-      <c r="C2" s="9">
-        <v>-69.872967000000003</v>
-      </c>
-      <c r="D2" s="9">
-        <v>1172</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="13">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1">
-        <f>65.91*10^7</f>
-        <v>659100000</v>
-      </c>
-      <c r="K2" s="1">
-        <f>1.2*10^7</f>
-        <v>12000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10">
-        <v>-19.340944</v>
-      </c>
-      <c r="C3" s="10">
-        <v>-69.727999999999994</v>
-      </c>
-      <c r="D3" s="10">
-        <v>1607</v>
-      </c>
-      <c r="E3" s="1">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2">
-        <f>74.48*10^7</f>
-        <v>744800000</v>
-      </c>
-      <c r="K3" s="2">
-        <f>2.33*10^7</f>
-        <v>23300000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="10">
-        <v>-19.340944</v>
-      </c>
-      <c r="C4" s="10">
-        <v>-69.727999999999994</v>
-      </c>
-      <c r="D4" s="10">
-        <v>1607</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2">
-        <f>91.1*10^7</f>
-        <v>911000000</v>
-      </c>
-      <c r="K4" s="2">
-        <f>1.3*10^7</f>
-        <v>13000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="10">
-        <v>-19.340944</v>
-      </c>
-      <c r="C5" s="10">
-        <v>-69.727999999999994</v>
-      </c>
-      <c r="D5" s="10">
-        <v>1607</v>
-      </c>
-      <c r="E5" s="1">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="13">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2">
-        <f>167.12*10^7</f>
-        <v>1671200000</v>
-      </c>
-      <c r="K5" s="2">
-        <f>3.65*10^7</f>
-        <v>36500000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="10">
-        <v>-19.336722000000002</v>
-      </c>
-      <c r="C6" s="10">
-        <v>-69.729611000000006</v>
-      </c>
-      <c r="D6" s="10">
-        <v>1604</v>
-      </c>
-      <c r="E6" s="1">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="13">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2">
-        <f>104.68*10^7</f>
-        <v>1046800000.0000001</v>
-      </c>
-      <c r="K6" s="2">
-        <f>2.24*10^7</f>
-        <v>22400000.000000004</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="9">
-        <v>-18.886583000000002</v>
-      </c>
-      <c r="C7" s="9">
-        <v>-69.699055999999999</v>
-      </c>
-      <c r="D7" s="9">
-        <v>2282</v>
-      </c>
-      <c r="E7" s="1">
-        <v>5</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2">
-        <f>269.89*10^7</f>
-        <v>2698900000</v>
-      </c>
-      <c r="K7" s="7">
-        <f>4.73*10^7</f>
-        <v>47300000.000000007</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="9">
-        <v>-18.886583000000002</v>
-      </c>
-      <c r="C8" s="9">
-        <v>-69.699055999999999</v>
-      </c>
-      <c r="D8" s="9">
-        <v>2282</v>
-      </c>
-      <c r="E8" s="1">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="13">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="2">
-        <f>246.53*10^7</f>
-        <v>2465300000</v>
-      </c>
-      <c r="K8" s="7">
-        <f>4.29*10^7</f>
-        <v>42900000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="9">
-        <v>-18.905639000000001</v>
-      </c>
-      <c r="C9" s="9">
-        <v>-69.954583</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1443</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="13">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="2">
-        <f>141.41*10^7</f>
-        <v>1414100000</v>
-      </c>
-      <c r="K9" s="7">
-        <f>2.52*10^7</f>
-        <v>25200000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="9">
-        <v>-18.905639000000001</v>
-      </c>
-      <c r="C10" s="9">
-        <v>-69.954583</v>
-      </c>
-      <c r="D10" s="9">
-        <v>1443</v>
-      </c>
-      <c r="E10" s="1">
-        <v>5</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="13">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="2">
-        <f>164.8*10^7</f>
-        <v>1648000000</v>
-      </c>
-      <c r="K10" s="7">
-        <f>2.84*10^7</f>
-        <v>28400000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="9">
-        <v>-18.852694</v>
-      </c>
-      <c r="C11" s="9">
-        <v>-69.657167000000001</v>
-      </c>
-      <c r="D11" s="9">
-        <v>2550</v>
-      </c>
-      <c r="E11" s="1">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="13">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="2">
-        <f>235*10^7</f>
-        <v>2350000000</v>
-      </c>
-      <c r="K11" s="7">
-        <f>4.04*10^7</f>
-        <v>40400000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="9">
-        <v>-20.704083000000001</v>
-      </c>
-      <c r="C12" s="9">
-        <v>-69.420833000000002</v>
-      </c>
-      <c r="D12" s="9">
-        <v>1084</v>
-      </c>
-      <c r="E12" s="1">
-        <v>5</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="13">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="2">
-        <f>90.19*10^7</f>
-        <v>901900000</v>
-      </c>
-      <c r="K12" s="7">
-        <f>1.97*10^7</f>
-        <v>19700000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="11">
-        <v>-19.786306</v>
-      </c>
-      <c r="C13" s="11">
-        <v>-69.682000000000002</v>
-      </c>
-      <c r="D13" s="11">
-        <v>1289</v>
-      </c>
-      <c r="E13" s="1">
-        <v>5</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="13">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="2">
-        <f>107.8*10^7</f>
-        <v>1078000000</v>
-      </c>
-      <c r="K13" s="2">
-        <f>2.77*10^7</f>
-        <v>27700000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="10">
-        <v>-19.786306</v>
-      </c>
-      <c r="C14" s="10">
-        <v>-69.682000000000002</v>
-      </c>
-      <c r="D14" s="10">
-        <v>1289</v>
-      </c>
-      <c r="E14" s="1">
-        <v>5</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="13">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="2">
-        <f>102.49*10^7</f>
-        <v>1024900000</v>
-      </c>
-      <c r="K14" s="2">
-        <f>2.48*10^7</f>
-        <v>24800000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="10">
-        <v>-19.786306</v>
-      </c>
-      <c r="C15" s="10">
-        <v>-69.682000000000002</v>
-      </c>
-      <c r="D15" s="10">
-        <v>1289</v>
-      </c>
-      <c r="E15" s="1">
-        <v>5</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="13">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="8">
-        <f>298.96*10^7</f>
-        <v>2989600000</v>
-      </c>
-      <c r="K15" s="2">
-        <f>3.2*10^7</f>
-        <v>32000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="10">
-        <v>-19.397832999999999</v>
-      </c>
-      <c r="C16" s="10">
-        <v>-69.880306000000004</v>
-      </c>
-      <c r="D16" s="10">
-        <v>1256</v>
-      </c>
-      <c r="E16" s="1">
-        <v>5</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="13">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="2">
-        <f>194.23*10^7</f>
-        <v>1942300000</v>
-      </c>
-      <c r="K16" s="2">
-        <f>4.67*10^7</f>
-        <v>46700000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="10">
-        <v>-19.397832999999999</v>
-      </c>
-      <c r="C17" s="10">
-        <v>-69.880306000000004</v>
-      </c>
-      <c r="D17" s="10">
-        <v>1256</v>
-      </c>
-      <c r="E17" s="1">
-        <v>5</v>
-      </c>
-      <c r="F17" s="1">
-        <v>2.74</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-      <c r="H17" s="13">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="2">
-        <f>310.26*10^7</f>
-        <v>3102600000</v>
-      </c>
-      <c r="K17" s="2">
-        <f>8.23*10^7</f>
-        <v>82300000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="10">
-        <v>-19.397832999999999</v>
-      </c>
-      <c r="C18" s="10">
-        <v>-69.880306000000004</v>
-      </c>
-      <c r="D18" s="10">
-        <v>1256</v>
-      </c>
-      <c r="E18" s="1">
-        <v>5</v>
-      </c>
-      <c r="F18" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-      <c r="H18" s="13">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="2">
-        <f>269.16*10^7</f>
-        <v>2691600000.0000005</v>
-      </c>
-      <c r="K18" s="2">
-        <f>6.18*10^7</f>
-        <v>61800000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="9">
-        <v>-19.522110999999999</v>
-      </c>
-      <c r="C19" s="9">
-        <v>-69.808333000000005</v>
-      </c>
-      <c r="D19" s="9">
-        <v>1312</v>
-      </c>
-      <c r="E19" s="1">
-        <v>5</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G19" s="1">
-        <v>1</v>
-      </c>
-      <c r="H19" s="13">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="2">
-        <f>277.15*10^7</f>
-        <v>2771500000</v>
-      </c>
-      <c r="K19" s="7">
-        <f>5.2*10^7</f>
-        <v>52000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="9">
-        <v>-19.522110999999999</v>
-      </c>
-      <c r="C20" s="9">
-        <v>-69.808333000000005</v>
-      </c>
-      <c r="D20" s="9">
-        <v>1312</v>
-      </c>
-      <c r="E20" s="1">
-        <v>5</v>
-      </c>
-      <c r="F20" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
-      <c r="H20" s="13">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="2">
-        <f>65.4*10^7</f>
-        <v>654000000</v>
-      </c>
-      <c r="K20" s="7">
-        <f>1.5*10^7</f>
-        <v>15000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="12">
-        <v>-18.503527999999999</v>
-      </c>
-      <c r="C21" s="12">
-        <v>-70.143305999999995</v>
-      </c>
-      <c r="D21" s="12">
-        <v>771</v>
-      </c>
-      <c r="E21" s="1">
-        <v>5</v>
-      </c>
-      <c r="F21" s="1">
-        <v>2.89</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-      <c r="H21" s="13">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="2">
-        <f>41.29*10^7</f>
-        <v>412900000</v>
-      </c>
-      <c r="K21" s="7">
-        <f>0.72*10^7</f>
-        <v>7200000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>